<commit_message>
errors in references for SITS 1.4.2-1
</commit_message>
<xml_diff>
--- a/model_comparison.xlsx
+++ b/model_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilbertocamara/sitsbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91FA867-57CD-E84C-BFC4-F52E5B563E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAC7058-37A7-C64C-8D78-DB0F38F963A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33680" yWindow="-240" windowWidth="23780" windowHeight="14960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="2720" windowWidth="34320" windowHeight="19720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rfor" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -426,11 +425,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A2" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1626,8 +1629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>